<commit_message>
refactor 5: KAF009: Update template file in
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF009_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF009_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\02.Projects\UK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF009_直行直帰の申請\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="直行直帰申請" sheetId="28" r:id="rId1"/>
@@ -68,14 +68,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -96,7 +96,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -333,89 +333,110 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
@@ -423,33 +444,6 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -458,6 +452,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -507,7 +507,7 @@
         <xdr:cNvPr id="37" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69C81286-F93A-473A-AA20-C0A2A391B4F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{69C81286-F93A-473A-AA20-C0A2A391B4F2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -515,8 +515,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2819400" y="219075"/>
-          <a:ext cx="555766" cy="522000"/>
+          <a:off x="3162300" y="219075"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -526,7 +526,7 @@
           <xdr:cNvPr id="38" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BCFB946-A7EF-4F04-A413-C73154115416}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9BCFB946-A7EF-4F04-A413-C73154115416}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -580,7 +580,7 @@
           <xdr:cNvPr id="39" name="直線コネクタ 38">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3CE6EF6-9B0A-4DE0-90FD-65B6A64CE0BB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B3CE6EF6-9B0A-4DE0-90FD-65B6A64CE0BB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -620,7 +620,7 @@
           <xdr:cNvPr id="40" name="直線コネクタ 39">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{661AF485-9BEE-4EC0-8925-5AA5C9235A46}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{661AF485-9BEE-4EC0-8925-5AA5C9235A46}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -660,7 +660,7 @@
           <xdr:cNvPr id="41" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F68F42E-5D18-4552-B3A2-7CEF370044C2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5F68F42E-5D18-4552-B3A2-7CEF370044C2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -716,7 +716,7 @@
           <xdr:cNvPr id="42" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FB2F163-D611-458F-8A66-1647BF606FF0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7FB2F163-D611-458F-8A66-1647BF606FF0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -772,7 +772,7 @@
           <xdr:cNvPr id="43" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A533F59B-2AFD-44A0-BFEB-AE7FFADAD04A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A533F59B-2AFD-44A0-BFEB-AE7FFADAD04A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -844,7 +844,7 @@
         <xdr:cNvPr id="44" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9385207D-2031-4A1F-A631-3DB96AAE9518}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9385207D-2031-4A1F-A631-3DB96AAE9518}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -852,8 +852,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3369247" y="219075"/>
-          <a:ext cx="555766" cy="522000"/>
+          <a:off x="3778822" y="219075"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -863,7 +863,7 @@
           <xdr:cNvPr id="45" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5F6CFDB-77A1-4E5C-A45A-9C39D6B75121}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F5F6CFDB-77A1-4E5C-A45A-9C39D6B75121}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -917,7 +917,7 @@
           <xdr:cNvPr id="46" name="直線コネクタ 45">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0B5AF4F-8494-4860-8430-E58B120D9B72}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0B5AF4F-8494-4860-8430-E58B120D9B72}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -957,7 +957,7 @@
           <xdr:cNvPr id="47" name="直線コネクタ 46">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B37F427-BE01-4E65-9D0B-40916F68644B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8B37F427-BE01-4E65-9D0B-40916F68644B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -997,7 +997,7 @@
           <xdr:cNvPr id="48" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73D3C67-383E-47BE-8996-A6F85D0C2EDB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73D3C67-383E-47BE-8996-A6F85D0C2EDB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1053,7 +1053,7 @@
           <xdr:cNvPr id="49" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88DD887D-8E1C-4657-8A27-3F85B4822B00}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{88DD887D-8E1C-4657-8A27-3F85B4822B00}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1109,7 +1109,7 @@
           <xdr:cNvPr id="50" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96BA1988-654E-4CD0-89E6-DFE027ADED1E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{96BA1988-654E-4CD0-89E6-DFE027ADED1E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1181,7 +1181,7 @@
         <xdr:cNvPr id="51" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5761DD66-EEF0-4C65-88CF-3A91AE49ADDB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5761DD66-EEF0-4C65-88CF-3A91AE49ADDB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1189,8 +1189,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3927140" y="219075"/>
-          <a:ext cx="546241" cy="522000"/>
+          <a:off x="4403390" y="219075"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1200,7 +1200,7 @@
           <xdr:cNvPr id="52" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7745DD80-0453-4BBE-B65C-CDC8D9694B1C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7745DD80-0453-4BBE-B65C-CDC8D9694B1C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1254,7 +1254,7 @@
           <xdr:cNvPr id="53" name="直線コネクタ 52">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{554A19A3-3420-4DA3-A8EE-64F1227DE14F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{554A19A3-3420-4DA3-A8EE-64F1227DE14F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1294,7 +1294,7 @@
           <xdr:cNvPr id="54" name="直線コネクタ 53">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9991D1EF-2B42-4FF0-AF07-9F0B8C65B636}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9991D1EF-2B42-4FF0-AF07-9F0B8C65B636}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1334,7 +1334,7 @@
           <xdr:cNvPr id="55" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CF45F56-65A5-4AF0-B2C3-588287D0363D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0CF45F56-65A5-4AF0-B2C3-588287D0363D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1390,7 +1390,7 @@
           <xdr:cNvPr id="56" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6888E981-D3C5-4DC0-BD3D-74249806953F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6888E981-D3C5-4DC0-BD3D-74249806953F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1446,7 +1446,7 @@
           <xdr:cNvPr id="57" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FDA955B-97EE-4A01-A9D6-F8D4DC7BEFA5}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2FDA955B-97EE-4A01-A9D6-F8D4DC7BEFA5}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1518,7 +1518,7 @@
         <xdr:cNvPr id="58" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{621CA222-C645-400B-A5DD-FBE09CBE117A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{621CA222-C645-400B-A5DD-FBE09CBE117A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1526,8 +1526,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4474148" y="219075"/>
-          <a:ext cx="555766" cy="522000"/>
+          <a:off x="5017073" y="219075"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1537,7 +1537,7 @@
           <xdr:cNvPr id="59" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2A997CB-09CF-4D44-8040-9191E806BA39}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B2A997CB-09CF-4D44-8040-9191E806BA39}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1591,7 +1591,7 @@
           <xdr:cNvPr id="60" name="直線コネクタ 59">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3689FC08-44E5-4BAC-B732-08CF2BD2C47B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3689FC08-44E5-4BAC-B732-08CF2BD2C47B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1631,7 +1631,7 @@
           <xdr:cNvPr id="61" name="直線コネクタ 60">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C955241F-CF19-4F68-A6ED-BF1A56D42519}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C955241F-CF19-4F68-A6ED-BF1A56D42519}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1671,7 +1671,7 @@
           <xdr:cNvPr id="62" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE00861C-6FC4-4421-A4FC-01B184123D38}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FE00861C-6FC4-4421-A4FC-01B184123D38}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1727,7 +1727,7 @@
           <xdr:cNvPr id="63" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{581A6BCC-6EB0-48D3-BFC1-EA2152F0ADF4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{581A6BCC-6EB0-48D3-BFC1-EA2152F0ADF4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1783,7 +1783,7 @@
           <xdr:cNvPr id="64" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28B76ED1-7F88-4DBC-BA01-91CF2571882C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{28B76ED1-7F88-4DBC-BA01-91CF2571882C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1855,7 +1855,7 @@
         <xdr:cNvPr id="100" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A704FCA9-D05C-4A2C-9ECF-C4C2EEE47717}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A704FCA9-D05C-4A2C-9ECF-C4C2EEE47717}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1863,8 +1863,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5032041" y="209550"/>
-          <a:ext cx="546241" cy="522000"/>
+          <a:off x="5641641" y="209550"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1874,7 +1874,7 @@
           <xdr:cNvPr id="101" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3394A81-9F5F-4614-8C35-7519B641669E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E3394A81-9F5F-4614-8C35-7519B641669E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1928,7 +1928,7 @@
           <xdr:cNvPr id="102" name="直線コネクタ 101">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC6E8B3B-82D2-47CC-9435-19EA0299F67F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DC6E8B3B-82D2-47CC-9435-19EA0299F67F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1968,7 +1968,7 @@
           <xdr:cNvPr id="103" name="直線コネクタ 102">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7014D014-A822-41A1-88E3-23DDDF993531}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7014D014-A822-41A1-88E3-23DDDF993531}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2008,7 +2008,7 @@
           <xdr:cNvPr id="104" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F744134E-34FA-4A85-9D2D-FA5E4E0D14F0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F744134E-34FA-4A85-9D2D-FA5E4E0D14F0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2064,7 +2064,7 @@
           <xdr:cNvPr id="105" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F2E3CE5-5BC8-49A7-9256-BABD3B31580D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F2E3CE5-5BC8-49A7-9256-BABD3B31580D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2110,7 +2110,7 @@
                 <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
                 <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
               </a:rPr>
-              <a:t> </a:t>
+              <a:t>  </a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -2120,7 +2120,7 @@
           <xdr:cNvPr id="106" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3B0439A-7D81-474D-A3D1-1B0AD51D58B7}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D3B0439A-7D81-474D-A3D1-1B0AD51D58B7}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2566,19 +2566,19 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="0.75" style="2" customWidth="1"/>
-    <col min="2" max="11" width="7.25" style="2" customWidth="1"/>
-    <col min="12" max="12" width="0.75" style="2" customWidth="1"/>
-    <col min="13" max="14" width="7.125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="1.375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="0.77734375" style="2" customWidth="1"/>
+    <col min="2" max="11" width="7.21875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="0.77734375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="7.109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="1.33203125" style="2" customWidth="1"/>
     <col min="17" max="17" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="2.5" style="2"/>
+    <col min="18" max="16384" width="2.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
@@ -2601,395 +2601,395 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="8"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="7"/>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="9.9499999999999993" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="13"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="12"/>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="13"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="12"/>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="16"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="16"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="16"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="16"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="3.75" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="21"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="20"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="90" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="47"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="45"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="3.75" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="26"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="25"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" ht="3.75" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="29"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="28"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="74.25" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="40"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="38"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="3.75" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="32"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="31"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1">
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="33"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1">
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1">
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1">
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1">
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1">
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1">
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1"/>
     <row r="33" ht="15" customHeight="1"/>
@@ -3001,7 +3001,7 @@
     <row r="39" ht="15" customHeight="1"/>
     <row r="40" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="C3:F3"/>
@@ -3010,6 +3010,10 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:K13"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>